<commit_message>
use cases fyrir a kröfur 4.0-4.4
</commit_message>
<xml_diff>
--- a/Hönnun/UseCases/Use_cases_A_WIP.xlsx
+++ b/Hönnun/UseCases/Use_cases_A_WIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Halli\Desktop\VLN1\VNL1-2022-HOPUR-28\Hönnun\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCEE173-74FB-4E49-B3BF-4A0435576FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98345196-AE18-4441-B4A9-9118D384901E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{D9CE7003-7C71-4049-AB61-1D7266533BEE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -75,20 +75,12 @@
   </si>
   <si>
     <t>Use Case Number</t>
-  </si>
-  <si>
-    <t>1. Input command to create new team
-2. Input command to cancel registration</t>
   </si>
   <si>
     <t>New team is registered
 Registration is cancelled</t>
   </si>
   <si>
-    <t>1. Input command to register new player
-2. Input command to cancel registration</t>
-  </si>
-  <si>
     <t>New player is registered
 registration is cancelled</t>
   </si>
@@ -100,9 +92,6 @@
   </si>
   <si>
     <t>Register new club</t>
-  </si>
-  <si>
-    <t>Register new league</t>
   </si>
   <si>
     <t>Admin</t>
@@ -144,10 +133,6 @@
 5. Confirm changes</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Select a club
-2. Select </t>
-  </si>
-  <si>
     <t>US2.1</t>
   </si>
   <si>
@@ -172,9 +157,6 @@
     <t>US4.0</t>
   </si>
   <si>
-    <t>Display League Table</t>
-  </si>
-  <si>
     <t>Admin, Captain, Player, Spectator</t>
   </si>
   <si>
@@ -182,10 +164,6 @@
   </si>
   <si>
     <t>Display Unplayed Matches</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In main menu
-</t>
   </si>
   <si>
     <t>US4.2</t>
@@ -228,10 +206,6 @@
     <t>Has admin rights</t>
   </si>
   <si>
-    <t>1. Select register new league option
-2. Input command to cancel registration</t>
-  </si>
-  <si>
     <t>Schedule new match</t>
   </si>
   <si>
@@ -247,11 +221,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>1. Select league page
-2. Select Schedule match
-3. Input command to cancel scheduling</t>
   </si>
   <si>
     <t>1. Select league page
@@ -278,12 +247,6 @@
 6. Review and confirm</t>
   </si>
   <si>
-    <t>1. Select league page
-2. Select match page
-3. Select reschedule match
-4. Input command to cancel rescheduling</t>
-  </si>
-  <si>
     <t>Has captain rights
 At least one match ongoing</t>
   </si>
@@ -296,11 +259,6 @@
 2. Select submit match result
 3. Input match all data from match
 4. Review and confirm</t>
-  </si>
-  <si>
-    <t>1. Select your open matches page
-2. Select submit match result
-3. Input command to cancel data submission</t>
   </si>
   <si>
     <t>Match data is submitted
@@ -315,10 +273,118 @@
 6. Review and confirm</t>
   </si>
   <si>
+    <t>1. Select a club
+2. Input team name
+3. Select players 
+4. Review and confirm</t>
+  </si>
+  <si>
+    <t>1. Input command to create new team
+2. Input command to cancel</t>
+  </si>
+  <si>
+    <t>New team is created
+Registration is cancelled</t>
+  </si>
+  <si>
+    <t>US1.0
+US1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Input command to register new player
+2. Input command to cancel </t>
+  </si>
+  <si>
+    <t>1. Select register new league option
+2. Input command to cancel</t>
+  </si>
+  <si>
+    <t>1. Select league page
+2. Select Schedule match
+3. Input command to cancel</t>
+  </si>
+  <si>
+    <t>1. Select league page
+2. Select match page
+3. Select reschedule match
+4. Input command to cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Select your open matches page
+2. Select submit match result
+3. Input command to cancel </t>
+  </si>
+  <si>
     <t>1. Select tournament page
 2. Select match page
 3. Select edit match results
-4. Input command to cancel result editing</t>
+4. Input command to cancel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Select "Unplayed Matches"
+2. Select tournament
+</t>
+  </si>
+  <si>
+    <t>US4.4</t>
+  </si>
+  <si>
+    <t>Display match data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Select "Unplayed Matches"
+2. Select tournament
+3. Select match
+</t>
+  </si>
+  <si>
+    <t>Match data is displayed
+Match data is not displayed</t>
+  </si>
+  <si>
+    <t>US4.1
+US4.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Select "Results"
+2. Repeat from main scenario step 2
+</t>
+  </si>
+  <si>
+    <t>Unplayed matches are displayed</t>
+  </si>
+  <si>
+    <t>1. Select "Results"
+2. Select tournament</t>
+  </si>
+  <si>
+    <t>Results are displayed</t>
+  </si>
+  <si>
+    <t>League table is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Display Division Table</t>
+  </si>
+  <si>
+    <t>1. Select "Division table"
+2. Select tournament</t>
+  </si>
+  <si>
+    <t>Create new divison</t>
+  </si>
+  <si>
+    <t>1. Select "Show Teams"</t>
+  </si>
+  <si>
+    <t>Teams are displayed</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -486,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -596,6 +662,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,7 +989,7 @@
   <dimension ref="B3:AW50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:G10"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,7 +1055,7 @@
       </c>
       <c r="C4" s="21"/>
       <c r="D4" s="22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
@@ -1083,7 +1159,7 @@
       </c>
       <c r="C6" s="21"/>
       <c r="D6" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="23"/>
@@ -1093,7 +1169,7 @@
       </c>
       <c r="J6" s="21"/>
       <c r="K6" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L6" s="23"/>
       <c r="M6" s="23"/>
@@ -1135,7 +1211,7 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1145,7 +1221,7 @@
       </c>
       <c r="J7" s="6"/>
       <c r="K7" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
@@ -1319,7 +1395,7 @@
       </c>
       <c r="C11" s="25"/>
       <c r="D11" s="25" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
@@ -1329,7 +1405,7 @@
       </c>
       <c r="J11" s="25"/>
       <c r="K11" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
@@ -1547,7 +1623,7 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="5" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
@@ -1639,7 +1715,7 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -1649,7 +1725,7 @@
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="5" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -1741,7 +1817,7 @@
       </c>
       <c r="J20" s="6"/>
       <c r="K20" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
@@ -1985,7 +2061,7 @@
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="22" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -1995,7 +2071,7 @@
       </c>
       <c r="J28" s="24"/>
       <c r="K28" s="22" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L28" s="23"/>
       <c r="M28" s="23"/>
@@ -2031,7 +2107,7 @@
       </c>
       <c r="C29" s="21"/>
       <c r="D29" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E29" s="23"/>
       <c r="F29" s="23"/>
@@ -2041,7 +2117,7 @@
       </c>
       <c r="J29" s="21"/>
       <c r="K29" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L29" s="23"/>
       <c r="M29" s="23"/>
@@ -2123,7 +2199,7 @@
       </c>
       <c r="C31" s="21"/>
       <c r="D31" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
@@ -2133,7 +2209,7 @@
       </c>
       <c r="J31" s="21"/>
       <c r="K31" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L31" s="23"/>
       <c r="M31" s="23"/>
@@ -2169,7 +2245,7 @@
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
@@ -2179,7 +2255,7 @@
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
@@ -2329,7 +2405,7 @@
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="25" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E36" s="25"/>
       <c r="F36" s="25"/>
@@ -2339,7 +2415,7 @@
       </c>
       <c r="J36" s="25"/>
       <c r="K36" s="25" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="L36" s="25"/>
       <c r="M36" s="25"/>
@@ -2527,7 +2603,7 @@
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="5" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -2537,7 +2613,7 @@
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="5" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
@@ -2611,7 +2687,7 @@
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
@@ -2621,7 +2697,7 @@
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="5" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
@@ -2733,7 +2809,7 @@
       </c>
       <c r="C46" s="25"/>
       <c r="D46" s="25" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E46" s="25"/>
       <c r="F46" s="25"/>
@@ -2742,7 +2818,9 @@
         <v>7</v>
       </c>
       <c r="J46" s="6"/>
-      <c r="K46" s="19"/>
+      <c r="K46" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
       <c r="N46" s="10"/>
@@ -2977,7 +3055,7 @@
   <dimension ref="B2:U49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+      <selection activeCell="D3" sqref="D3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2988,7 +3066,7 @@
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
@@ -2998,7 +3076,7 @@
       </c>
       <c r="J2" s="24"/>
       <c r="K2" s="22" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
@@ -3008,7 +3086,7 @@
       </c>
       <c r="Q2" s="24"/>
       <c r="R2" s="22" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="S2" s="23"/>
       <c r="T2" s="23"/>
@@ -3020,7 +3098,7 @@
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="22" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
@@ -3030,7 +3108,7 @@
       </c>
       <c r="J3" s="21"/>
       <c r="K3" s="22" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
@@ -3040,7 +3118,7 @@
       </c>
       <c r="Q3" s="21"/>
       <c r="R3" s="22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="S3" s="23"/>
       <c r="T3" s="23"/>
@@ -3084,7 +3162,7 @@
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
@@ -3094,7 +3172,7 @@
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="23"/>
@@ -3104,7 +3182,7 @@
       </c>
       <c r="Q5" s="21"/>
       <c r="R5" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="S5" s="23"/>
       <c r="T5" s="23"/>
@@ -3116,7 +3194,7 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -3126,7 +3204,7 @@
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
@@ -3136,7 +3214,7 @@
       </c>
       <c r="Q6" s="6"/>
       <c r="R6" s="5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
@@ -3208,7 +3286,7 @@
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="25" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
@@ -3218,7 +3296,7 @@
       </c>
       <c r="J10" s="25"/>
       <c r="K10" s="25" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
@@ -3228,7 +3306,7 @@
       </c>
       <c r="Q10" s="29"/>
       <c r="R10" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="S10" s="34"/>
       <c r="T10" s="34"/>
@@ -3332,7 +3410,7 @@
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="25" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="S15" s="25"/>
       <c r="T15" s="25"/>
@@ -3350,7 +3428,7 @@
       </c>
       <c r="J16" s="25"/>
       <c r="K16" s="25" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -3368,7 +3446,7 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="5" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -3412,7 +3490,7 @@
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -3422,7 +3500,7 @@
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -3432,7 +3510,7 @@
       </c>
       <c r="Q19" s="6"/>
       <c r="R19" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="S19" s="9"/>
       <c r="T19" s="9"/>
@@ -3484,7 +3562,7 @@
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="19" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
@@ -3494,7 +3572,7 @@
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
@@ -3504,7 +3582,7 @@
       </c>
       <c r="Q22" s="6"/>
       <c r="R22" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="S22" s="9"/>
       <c r="T22" s="9"/>
@@ -3736,7 +3814,7 @@
   <dimension ref="B2:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3747,7 +3825,7 @@
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
@@ -3757,7 +3835,7 @@
       </c>
       <c r="J2" s="24"/>
       <c r="K2" s="22" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
@@ -3769,7 +3847,7 @@
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
@@ -3779,7 +3857,7 @@
       </c>
       <c r="J3" s="21"/>
       <c r="K3" s="22" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
@@ -3813,7 +3891,7 @@
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
@@ -3823,7 +3901,7 @@
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="23"/>
@@ -3835,7 +3913,7 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -3845,7 +3923,7 @@
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
@@ -3899,7 +3977,7 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="5" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
@@ -3909,7 +3987,7 @@
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="L10" s="34"/>
       <c r="M10" s="34"/>
@@ -3963,7 +4041,7 @@
       </c>
       <c r="C14" s="25"/>
       <c r="D14" s="25" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
@@ -4001,7 +4079,7 @@
       </c>
       <c r="J16" s="25"/>
       <c r="K16" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
@@ -4013,7 +4091,7 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -4059,7 +4137,7 @@
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -4101,7 +4179,7 @@
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="19" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
@@ -4160,21 +4238,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{748E5D56-74C3-4540-B300-BA6D116ACDA7}">
-  <dimension ref="B2:N49"/>
+  <dimension ref="B2:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="22" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
@@ -4184,19 +4262,29 @@
       </c>
       <c r="J2" s="24"/>
       <c r="K2" s="22" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
       <c r="N2" s="24"/>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="24"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B3" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="22" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
@@ -4206,13 +4294,23 @@
       </c>
       <c r="J3" s="21"/>
       <c r="K3" s="22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
       <c r="N3" s="24"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="24"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B4" s="26" t="s">
         <v>1</v>
       </c>
@@ -4233,14 +4331,24 @@
       <c r="L4" s="23"/>
       <c r="M4" s="23"/>
       <c r="N4" s="24"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P4" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="22">
+        <v>1</v>
+      </c>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="24"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B5" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
@@ -4250,19 +4358,29 @@
       </c>
       <c r="J5" s="21"/>
       <c r="K5" s="22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="23"/>
       <c r="N5" s="24"/>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="24"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="5" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
@@ -4271,14 +4389,22 @@
         <v>3</v>
       </c>
       <c r="J6" s="6"/>
-      <c r="K6" s="5" t="s">
-        <v>41</v>
-      </c>
+      <c r="K6" s="5"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="10"/>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="10"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
@@ -4291,8 +4417,14 @@
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="18"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P7" s="14"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="18"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B8" s="14"/>
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
@@ -4305,8 +4437,14 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="18"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="18"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="11"/>
@@ -4319,13 +4457,21 @@
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
       <c r="N9" s="13"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P9" s="7"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="13"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B10" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>85</v>
+      </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
@@ -4333,12 +4479,24 @@
         <v>4</v>
       </c>
       <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
+      <c r="K10" s="25" t="s">
+        <v>70</v>
+      </c>
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P10" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
@@ -4351,8 +4509,14 @@
       <c r="L11" s="25"/>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B12" s="25"/>
       <c r="C12" s="25"/>
       <c r="D12" s="25"/>
@@ -4365,8 +4529,14 @@
       <c r="L12" s="25"/>
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B13" s="25"/>
       <c r="C13" s="25"/>
       <c r="D13" s="25"/>
@@ -4379,8 +4549,14 @@
       <c r="L13" s="25"/>
       <c r="M13" s="25"/>
       <c r="N13" s="25"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
@@ -4393,8 +4569,14 @@
       <c r="L14" s="25"/>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
@@ -4407,8 +4589,14 @@
       <c r="L15" s="25"/>
       <c r="M15" s="25"/>
       <c r="N15" s="25"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
@@ -4421,8 +4609,14 @@
       <c r="L16" s="25"/>
       <c r="M16" s="25"/>
       <c r="N16" s="25"/>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
@@ -4435,8 +4629,14 @@
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
       <c r="N17" s="25"/>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
@@ -4453,8 +4653,18 @@
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="10"/>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="10"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="11"/>
@@ -4467,13 +4677,21 @@
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
       <c r="N19" s="13"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P19" s="7"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="13"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>86</v>
+      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="10"/>
@@ -4481,12 +4699,24 @@
         <v>6</v>
       </c>
       <c r="J20" s="6"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5" t="s">
+        <v>77</v>
+      </c>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="10"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="10"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
       <c r="D21" s="16"/>
@@ -4499,8 +4729,14 @@
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
       <c r="N21" s="18"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P21" s="14"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="16"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="18"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="11"/>
@@ -4513,8 +4749,14 @@
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
       <c r="N22" s="13"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P22" s="7"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="13"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>7</v>
       </c>
@@ -4527,12 +4769,24 @@
         <v>7</v>
       </c>
       <c r="J23" s="6"/>
-      <c r="K23" s="19"/>
+      <c r="K23" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="10"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P23" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="10"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="11"/>
@@ -4545,14 +4799,20 @@
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
       <c r="N24" s="13"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="P24" s="7"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="13"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B27" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="22" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E27" s="23"/>
       <c r="F27" s="23"/>
@@ -4562,19 +4822,19 @@
       </c>
       <c r="J27" s="24"/>
       <c r="K27" s="22" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="L27" s="23"/>
       <c r="M27" s="23"/>
       <c r="N27" s="24"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B28" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E28" s="23"/>
       <c r="F28" s="23"/>
@@ -4584,13 +4844,13 @@
       </c>
       <c r="J28" s="21"/>
       <c r="K28" s="22" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="L28" s="23"/>
       <c r="M28" s="23"/>
       <c r="N28" s="24"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B29" s="26" t="s">
         <v>1</v>
       </c>
@@ -4612,13 +4872,13 @@
       <c r="M29" s="23"/>
       <c r="N29" s="24"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B30" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C30" s="21"/>
       <c r="D30" s="22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E30" s="23"/>
       <c r="F30" s="23"/>
@@ -4628,19 +4888,19 @@
       </c>
       <c r="J30" s="21"/>
       <c r="K30" s="22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="L30" s="23"/>
       <c r="M30" s="23"/>
       <c r="N30" s="24"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="5" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
@@ -4650,13 +4910,16 @@
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="5" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="10"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="Q31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
       <c r="D32" s="16"/>
@@ -4698,23 +4961,27 @@
       <c r="M34" s="12"/>
       <c r="N34" s="13"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
+      <c r="D35" s="25" t="s">
+        <v>78</v>
+      </c>
       <c r="E35" s="25"/>
       <c r="F35" s="25"/>
       <c r="G35" s="25"/>
-      <c r="I35" s="25" t="s">
+      <c r="I35" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L35" s="34"/>
+      <c r="M35" s="34"/>
+      <c r="N35" s="6"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" s="25"/>
@@ -4723,12 +4990,12 @@
       <c r="E36" s="25"/>
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="8"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" s="25"/>
@@ -4737,12 +5004,16 @@
       <c r="E37" s="25"/>
       <c r="F37" s="25"/>
       <c r="G37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
+      <c r="I37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="6"/>
+      <c r="K37" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="10"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" s="25"/>
@@ -4751,12 +5022,12 @@
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
       <c r="G38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="18"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" s="25"/>
@@ -4765,12 +5036,12 @@
       <c r="E39" s="25"/>
       <c r="F39" s="25"/>
       <c r="G39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="18"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" s="25"/>
@@ -4779,12 +5050,12 @@
       <c r="E40" s="25"/>
       <c r="F40" s="25"/>
       <c r="G40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B41" s="25"/>
@@ -4793,12 +5064,12 @@
       <c r="E41" s="25"/>
       <c r="F41" s="25"/>
       <c r="G41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="37"/>
+      <c r="K41" s="37"/>
+      <c r="L41" s="37"/>
+      <c r="M41" s="37"/>
+      <c r="N41" s="37"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B42" s="25"/>
@@ -4807,12 +5078,12 @@
       <c r="E42" s="25"/>
       <c r="F42" s="25"/>
       <c r="G42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="37"/>
+      <c r="K42" s="37"/>
+      <c r="L42" s="37"/>
+      <c r="M42" s="37"/>
+      <c r="N42" s="37"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B43" s="5" t="s">
@@ -4823,14 +5094,12 @@
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
       <c r="G43" s="10"/>
-      <c r="I43" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J43" s="6"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="10"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="39"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="39"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B44" s="7"/>
@@ -4839,30 +5108,30 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
       <c r="G44" s="13"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="13"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="39"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B45" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C45" s="6"/>
-      <c r="D45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>79</v>
+      </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
       <c r="G45" s="10"/>
-      <c r="I45" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J45" s="6"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="10"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
+      <c r="K45" s="40"/>
+      <c r="L45" s="40"/>
+      <c r="M45" s="40"/>
+      <c r="N45" s="40"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B46" s="14"/>
@@ -4871,12 +5140,12 @@
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="17"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="18"/>
+      <c r="I46" s="40"/>
+      <c r="J46" s="40"/>
+      <c r="K46" s="40"/>
+      <c r="L46" s="40"/>
+      <c r="M46" s="40"/>
+      <c r="N46" s="40"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B47" s="7"/>
@@ -4885,30 +5154,30 @@
       <c r="E47" s="12"/>
       <c r="F47" s="12"/>
       <c r="G47" s="13"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="13"/>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
+      <c r="K47" s="40"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="40"/>
+      <c r="N47" s="40"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B48" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C48" s="6"/>
-      <c r="D48" s="19"/>
+      <c r="D48" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
       <c r="G48" s="10"/>
-      <c r="I48" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J48" s="6"/>
-      <c r="K48" s="19"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="10"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="39"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="39"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B49" s="7"/>
@@ -4917,15 +5186,33 @@
       <c r="E49" s="12"/>
       <c r="F49" s="12"/>
       <c r="G49" s="13"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="13"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="39"/>
+      <c r="N49" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="90">
+    <mergeCell ref="P18:Q19"/>
+    <mergeCell ref="R18:U19"/>
+    <mergeCell ref="P20:Q22"/>
+    <mergeCell ref="R20:U22"/>
+    <mergeCell ref="P23:Q24"/>
+    <mergeCell ref="R23:U24"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="P6:Q9"/>
+    <mergeCell ref="R6:U9"/>
+    <mergeCell ref="P10:Q17"/>
+    <mergeCell ref="R10:U17"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:U4"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="B2:C2"/>
@@ -4984,16 +5271,16 @@
     <mergeCell ref="K31:N34"/>
     <mergeCell ref="B35:C42"/>
     <mergeCell ref="D35:G42"/>
-    <mergeCell ref="I35:J42"/>
-    <mergeCell ref="K35:N42"/>
     <mergeCell ref="B43:C44"/>
     <mergeCell ref="D43:G44"/>
     <mergeCell ref="I43:J44"/>
     <mergeCell ref="K43:N44"/>
+    <mergeCell ref="K35:N36"/>
+    <mergeCell ref="I35:J36"/>
     <mergeCell ref="B45:C47"/>
     <mergeCell ref="D45:G47"/>
-    <mergeCell ref="I45:J47"/>
-    <mergeCell ref="K45:N47"/>
+    <mergeCell ref="I37:J39"/>
+    <mergeCell ref="K37:N39"/>
     <mergeCell ref="B48:C49"/>
     <mergeCell ref="D48:G49"/>
     <mergeCell ref="I48:J49"/>

</xml_diff>